<commit_message>
get 3 SSA tests working; properly handle SSA submodel with total propensities == 0: if the simulation has 1 submodel and the total propensities are 0 suspend SSA by scheduling an event for infinity, which allows all other activities, like checkpointing to finish; try to use the wc_lang SBML Importer to create wc_lang test models from the SBML test suite but it fails on the first 150 models in the suite because their components lack sufficient units; improve plotting of debugging runs
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/stochastic/00003/00003-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/stochastic/00003/00003-wc_lang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-22540" yWindow="6680" windowWidth="22280" windowHeight="12020" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="-20980" yWindow="8380" windowWidth="20580" windowHeight="12940" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4692,9 +4692,6 @@
     <t>!Intention type</t>
   </si>
   <si>
-    <t>test_case_00001</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -4807,6 +4804,9 @@
   </si>
   <si>
     <t>Volume not used</t>
+  </si>
+  <si>
+    <t>test_case_00003</t>
   </si>
 </sst>
 </file>
@@ -6095,22 +6095,22 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6123,22 +6123,22 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>181</v>
-      </c>
       <c r="D5" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6339,7 +6339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
@@ -6406,21 +6406,21 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6430,21 +6430,21 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -7331,7 +7331,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -7395,7 +7395,7 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -7406,19 +7406,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" s="8"/>
       <c r="D4" s="24">
@@ -7428,12 +7428,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5" s="8"/>
       <c r="D5" s="24">
@@ -7443,7 +7443,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -8267,11 +8267,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -8302,7 +8302,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8320,7 +8320,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -9985,7 +9985,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -10017,7 +10017,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10049,7 +10049,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10313,13 +10313,13 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>182</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="3"/>
@@ -10587,24 +10587,24 @@
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" t="s">
         <v>156</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>158</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -10613,10 +10613,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -10626,7 +10626,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U4" s="3"/>
     </row>
@@ -11018,10 +11018,10 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -11034,13 +11034,13 @@
         <v>0</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N4" s="3"/>
     </row>
@@ -11280,17 +11280,17 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -11519,14 +11519,14 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" s="18">
         <v>100</v>
@@ -11535,7 +11535,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>

</xml_diff>